<commit_message>
Actualización - Formulación de control, Junta semanal (Semana 3) y primer boceto diagrama electrico
</commit_message>
<xml_diff>
--- a/Formato_Junta_Semanal.xlsx
+++ b/Formato_Junta_Semanal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CETI\Proyecto\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5093237B-1402-4301-8209-0FD3DBBD3021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F784CCD-69E6-40DE-A9FA-F4264DA05256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato Juna Semanal" sheetId="3" r:id="rId1"/>
@@ -672,6 +672,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -691,6 +719,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -706,36 +737,11 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -743,14 +749,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -982,65 +982,65 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:14" ht="15.75">
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="51"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="24"/>
     </row>
     <row r="6" spans="3:14" ht="15.75">
       <c r="C6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="51"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="24"/>
     </row>
     <row r="7" spans="3:14" ht="15.75">
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52" t="s">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="51"/>
-    </row>
-    <row r="8" spans="3:14" ht="31.5">
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="24"/>
+    </row>
+    <row r="8" spans="3:14" ht="15.75">
       <c r="C8" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="51"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="16" t="s">
         <v>54</v>
       </c>
@@ -1050,135 +1050,135 @@
       <c r="J8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="55"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="42"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="27"/>
     </row>
     <row r="9" spans="3:14" ht="15.75">
       <c r="C9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="51"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="16"/>
       <c r="I9" s="14"/>
       <c r="J9" s="18"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="45"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="30"/>
     </row>
     <row r="10" spans="3:14" ht="15.75">
       <c r="C10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="51"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="16"/>
       <c r="I10" s="14"/>
       <c r="J10" s="18"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="45"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="3:14" ht="15.75">
       <c r="C11" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="51"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="16"/>
       <c r="I11" s="14"/>
       <c r="J11" s="18"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="45"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="3:14" ht="15.75">
       <c r="C12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
       <c r="H12" s="16"/>
       <c r="I12" s="14"/>
       <c r="J12" s="18"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="45"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="3:14" ht="15.75">
       <c r="C13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="16"/>
       <c r="I13" s="14"/>
       <c r="J13" s="18"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="45"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="30"/>
     </row>
     <row r="14" spans="3:14" ht="15.75">
       <c r="C14" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="24"/>
       <c r="H14" s="16"/>
       <c r="I14" s="14"/>
       <c r="J14" s="18"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="48"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="33"/>
     </row>
     <row r="15" spans="3:14" ht="15.75">
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="52" t="s">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="51"/>
-    </row>
-    <row r="16" spans="3:14" ht="31.5">
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="24"/>
+    </row>
+    <row r="16" spans="3:14" ht="15.75">
       <c r="C16" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="52" t="s">
+      <c r="D16" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="51"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="16" t="s">
         <v>54</v>
       </c>
@@ -1188,151 +1188,151 @@
       <c r="J16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="40"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="42"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="27"/>
     </row>
     <row r="17" spans="3:14" ht="15.75">
       <c r="C17" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="51"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="16"/>
       <c r="I17" s="14"/>
       <c r="J17" s="18"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
-      <c r="N17" s="45"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="30"/>
     </row>
     <row r="18" spans="3:14" ht="15.75">
       <c r="C18" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="16"/>
       <c r="I18" s="14"/>
       <c r="J18" s="18"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="45"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="30"/>
     </row>
     <row r="19" spans="3:14" ht="15.75">
       <c r="C19" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="49"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="16"/>
       <c r="I19" s="14"/>
       <c r="J19" s="18"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="45"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="30"/>
     </row>
     <row r="20" spans="3:14" ht="15.75">
       <c r="C20" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="49"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="51"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="16"/>
       <c r="I20" s="14"/>
       <c r="J20" s="18"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="45"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="30"/>
     </row>
     <row r="21" spans="3:14" ht="15.75">
       <c r="C21" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="49"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="16"/>
       <c r="I21" s="14"/>
       <c r="J21" s="18"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="45"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="30"/>
     </row>
     <row r="22" spans="3:14" ht="15.75">
       <c r="C22" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="51"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="24"/>
       <c r="H22" s="16"/>
       <c r="I22" s="14"/>
       <c r="J22" s="18"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="45"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="30"/>
     </row>
     <row r="23" spans="3:14" ht="15.75">
       <c r="C23" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="49"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="51"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="16"/>
       <c r="I23" s="14"/>
       <c r="J23" s="18"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="48"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="33"/>
     </row>
     <row r="24" spans="3:14" ht="15.75">
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="52" t="s">
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L24" s="50"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="51"/>
-    </row>
-    <row r="25" spans="3:14" ht="31.5">
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="24"/>
+    </row>
+    <row r="25" spans="3:14" ht="15.75">
       <c r="C25" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="52" t="s">
+      <c r="D25" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="51"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="24"/>
       <c r="H25" s="16" t="s">
         <v>54</v>
       </c>
@@ -1342,103 +1342,103 @@
       <c r="J25" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K25" s="53"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="42"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="27"/>
     </row>
     <row r="26" spans="3:14" ht="15.75">
       <c r="C26" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="49"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="51"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="24"/>
       <c r="H26" s="16"/>
       <c r="I26" s="14"/>
       <c r="J26" s="18"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="45"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="30"/>
     </row>
     <row r="27" spans="3:14" ht="15.75">
       <c r="C27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="49"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="51"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="24"/>
       <c r="H27" s="16"/>
       <c r="I27" s="14"/>
       <c r="J27" s="18"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="45"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="30"/>
     </row>
     <row r="28" spans="3:14" ht="15.75">
       <c r="C28" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="49"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="51"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="16"/>
       <c r="I28" s="14"/>
       <c r="J28" s="18"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="45"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="30"/>
     </row>
     <row r="29" spans="3:14" ht="15.75">
       <c r="C29" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="49"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="51"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="24"/>
       <c r="H29" s="16"/>
       <c r="I29" s="14"/>
       <c r="J29" s="18"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="48"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="33"/>
     </row>
     <row r="30" spans="3:14" ht="15.75">
-      <c r="C30" s="52" t="s">
+      <c r="C30" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="52" t="s">
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L30" s="50"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="51"/>
-    </row>
-    <row r="31" spans="3:14" ht="31.5">
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="24"/>
+    </row>
+    <row r="31" spans="3:14" ht="15.75">
       <c r="C31" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="52" t="s">
+      <c r="D31" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="51"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="24"/>
       <c r="H31" s="16" t="s">
         <v>54</v>
       </c>
@@ -1448,68 +1448,45 @@
       <c r="J31" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K31" s="53"/>
-      <c r="L31" s="41"/>
-      <c r="M31" s="41"/>
-      <c r="N31" s="42"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="27"/>
     </row>
     <row r="32" spans="3:14" ht="15.75">
       <c r="C32" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="49"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="51"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="24"/>
       <c r="H32" s="16"/>
       <c r="I32" s="14"/>
       <c r="J32" s="18"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="44"/>
-      <c r="M32" s="44"/>
-      <c r="N32" s="45"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="30"/>
     </row>
     <row r="33" spans="3:14" ht="15.75">
       <c r="C33" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="49"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="51"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
       <c r="H33" s="16"/>
       <c r="I33" s="14"/>
       <c r="J33" s="18"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="48"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="D6:N6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="K8:N14"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="C15:J15"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="K16:N23"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D23:G23"/>
     <mergeCell ref="D31:G31"/>
     <mergeCell ref="K31:N33"/>
     <mergeCell ref="D32:G32"/>
@@ -1524,6 +1501,29 @@
     <mergeCell ref="D26:G26"/>
     <mergeCell ref="D27:G27"/>
     <mergeCell ref="D28:G28"/>
+    <mergeCell ref="C15:J15"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="K16:N23"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="D6:N6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="K8:N14"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J9:J14 J17:J23 J26:J29 J32:J33" xr:uid="{54633C2B-776C-4BE2-9795-9DCB46755862}">
@@ -1568,146 +1568,146 @@
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="23"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="39"/>
     </row>
     <row r="4" spans="3:16" ht="65.25" customHeight="1">
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="23"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="39"/>
     </row>
     <row r="5" spans="3:16" ht="32.25" customHeight="1">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="39"/>
       <c r="K5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="36"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="23"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="39"/>
     </row>
     <row r="6" spans="3:16" ht="24.75" customHeight="1">
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="55">
         <v>45727</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="55">
         <v>45788</v>
       </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="23"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="39"/>
       <c r="K6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="36"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="39"/>
     </row>
     <row r="7" spans="3:16" ht="14.25" customHeight="1"/>
     <row r="8" spans="3:16" ht="14.25" customHeight="1"/>
     <row r="9" spans="3:16" ht="25.5" customHeight="1">
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="23"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="39"/>
     </row>
     <row r="10" spans="3:16" ht="20.25" customHeight="1">
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="23"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="39"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
     </row>
     <row r="11" spans="3:16" ht="14.25" customHeight="1">
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="21" t="s">
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="23"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="39"/>
     </row>
     <row r="12" spans="3:16" ht="14.25" customHeight="1">
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="39"/>
       <c r="H12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1717,21 +1717,21 @@
       <c r="J12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="35"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="26"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="42"/>
     </row>
     <row r="13" spans="3:16" ht="14.25" customHeight="1">
       <c r="C13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="6"/>
       <c r="I13" s="5" t="s">
         <v>77</v>
@@ -1739,21 +1739,21 @@
       <c r="J13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="27"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="29"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="45"/>
     </row>
     <row r="14" spans="3:16" ht="14.25" customHeight="1">
       <c r="C14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
       <c r="H14" s="6"/>
       <c r="I14" s="5" t="s">
         <v>77</v>
@@ -1761,21 +1761,21 @@
       <c r="J14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K14" s="27"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="29"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="45"/>
     </row>
     <row r="15" spans="3:16" ht="14.25" customHeight="1">
       <c r="C15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="39"/>
       <c r="H15" s="6"/>
       <c r="I15" s="5" t="s">
         <v>77</v>
@@ -1783,21 +1783,21 @@
       <c r="J15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K15" s="27"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="29"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="45"/>
     </row>
     <row r="16" spans="3:16" ht="14.25" customHeight="1">
       <c r="C16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="39"/>
       <c r="H16" s="6"/>
       <c r="I16" s="5" t="s">
         <v>78</v>
@@ -1805,21 +1805,21 @@
       <c r="J16" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K16" s="27"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="29"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="44"/>
+      <c r="N16" s="45"/>
     </row>
     <row r="17" spans="3:14" ht="14.25" customHeight="1">
       <c r="C17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="23"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="6"/>
       <c r="I17" s="5" t="s">
         <v>78</v>
@@ -1827,39 +1827,39 @@
       <c r="J17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K17" s="30"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="32"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="48"/>
     </row>
     <row r="18" spans="3:14" ht="14.25" customHeight="1">
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="21" t="s">
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="23"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="39"/>
     </row>
     <row r="19" spans="3:14" ht="14.25" customHeight="1">
       <c r="C19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="23"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="39"/>
       <c r="H19" s="5" t="s">
         <v>15</v>
       </c>
@@ -1869,21 +1869,21 @@
       <c r="J19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="34"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="26"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="42"/>
     </row>
     <row r="20" spans="3:14" ht="14.25" customHeight="1">
       <c r="C20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="23"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="39"/>
       <c r="H20" s="6"/>
       <c r="I20" s="5" t="s">
         <v>75</v>
@@ -1891,21 +1891,21 @@
       <c r="J20" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="27"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="29"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="45"/>
     </row>
     <row r="21" spans="3:14" ht="14.25" customHeight="1">
       <c r="C21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="23"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="39"/>
       <c r="H21" s="6"/>
       <c r="I21" s="5" t="s">
         <v>75</v>
@@ -1913,21 +1913,21 @@
       <c r="J21" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K21" s="27"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="29"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="45"/>
     </row>
     <row r="22" spans="3:14" ht="14.25" customHeight="1">
       <c r="C22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="23"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="39"/>
       <c r="H22" s="6"/>
       <c r="I22" s="5" t="s">
         <v>75</v>
@@ -1935,21 +1935,21 @@
       <c r="J22" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K22" s="27"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="29"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="45"/>
     </row>
     <row r="23" spans="3:14" ht="14.25" customHeight="1">
       <c r="C23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="23"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
       <c r="H23" s="6" t="s">
         <v>18</v>
       </c>
@@ -1959,21 +1959,21 @@
       <c r="J23" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K23" s="27"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="29"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="45"/>
     </row>
     <row r="24" spans="3:14" ht="14.25" customHeight="1">
       <c r="C24" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="23"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="39"/>
       <c r="H24" s="6"/>
       <c r="I24" s="5" t="s">
         <v>78</v>
@@ -1981,21 +1981,21 @@
       <c r="J24" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K24" s="27"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="29"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="45"/>
     </row>
     <row r="25" spans="3:14" ht="14.25" customHeight="1">
       <c r="C25" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="23"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="39"/>
       <c r="H25" s="6" t="s">
         <v>24</v>
       </c>
@@ -2005,21 +2005,21 @@
       <c r="J25" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K25" s="27"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="29"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="45"/>
     </row>
     <row r="26" spans="3:14" ht="14.25" customHeight="1">
       <c r="C26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="23"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="39"/>
       <c r="H26" s="6"/>
       <c r="I26" s="5" t="s">
         <v>75</v>
@@ -2027,39 +2027,39 @@
       <c r="J26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K26" s="30"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="32"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="48"/>
     </row>
     <row r="27" spans="3:14" ht="14.25" customHeight="1">
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="21" t="s">
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="23"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="39"/>
     </row>
     <row r="28" spans="3:14" ht="14.25" customHeight="1">
       <c r="C28" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="23"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="39"/>
       <c r="H28" s="5" t="s">
         <v>15</v>
       </c>
@@ -2069,21 +2069,21 @@
       <c r="J28" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="24"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="26"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="42"/>
     </row>
     <row r="29" spans="3:14" ht="14.25" customHeight="1">
       <c r="C29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="23"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="39"/>
       <c r="H29" s="6" t="s">
         <v>46</v>
       </c>
@@ -2093,21 +2093,21 @@
       <c r="J29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="K29" s="27"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="29"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="45"/>
     </row>
     <row r="30" spans="3:14" ht="14.25" customHeight="1">
       <c r="C30" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="23"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="39"/>
       <c r="H30" s="6" t="s">
         <v>49</v>
       </c>
@@ -2117,17 +2117,17 @@
       <c r="J30" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="K30" s="30"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="32"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="48"/>
     </row>
     <row r="31" spans="3:14" ht="14.25" customHeight="1">
       <c r="C31" s="4"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
       <c r="H31" s="8"/>
       <c r="I31" s="4"/>
       <c r="J31" s="9"/>
@@ -2138,10 +2138,10 @@
     </row>
     <row r="32" spans="3:14" ht="14.25" customHeight="1">
       <c r="C32" s="4"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
       <c r="H32" s="8"/>
       <c r="I32" s="4"/>
       <c r="J32" s="9"/>
@@ -2152,10 +2152,10 @@
     </row>
     <row r="33" spans="3:14" ht="14.25" customHeight="1">
       <c r="C33" s="4"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
       <c r="H33" s="8"/>
       <c r="I33" s="4"/>
       <c r="J33" s="9"/>
@@ -2166,10 +2166,10 @@
     </row>
     <row r="34" spans="3:14" ht="14.25" customHeight="1">
       <c r="C34" s="4"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
       <c r="H34" s="8"/>
       <c r="I34" s="4"/>
       <c r="J34" s="9"/>
@@ -2180,10 +2180,10 @@
     </row>
     <row r="35" spans="3:14" ht="14.25" customHeight="1">
       <c r="C35" s="4"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="9"/>
@@ -3302,17 +3302,24 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C27:J27"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="K28:N30"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="D3:N3"/>
+    <mergeCell ref="D4:N4"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="D10:N10"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="K12:N17"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
     <mergeCell ref="D24:G24"/>
     <mergeCell ref="D25:G25"/>
     <mergeCell ref="C18:J18"/>
@@ -3324,24 +3331,17 @@
     <mergeCell ref="D23:G23"/>
     <mergeCell ref="D26:G26"/>
     <mergeCell ref="D19:G19"/>
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="D10:N10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="K12:N17"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D3:N3"/>
-    <mergeCell ref="D4:N4"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="K28:N30"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D30:G30"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I13:I17 I20:I26 I29:I30" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -3388,19 +3388,19 @@
       <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="51"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="24"/>
     </row>
     <row r="4" spans="3:14" ht="14.25" customHeight="1">
       <c r="C4" s="12"/>
@@ -3431,67 +3431,67 @@
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="3:14" ht="27.75" customHeight="1">
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="51"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="24"/>
     </row>
     <row r="7" spans="3:14" ht="25.5" customHeight="1">
       <c r="C7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="51"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="24"/>
     </row>
     <row r="8" spans="3:14" ht="14.25" customHeight="1">
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="52" t="s">
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="51"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="24"/>
     </row>
     <row r="9" spans="3:14" ht="14.25" customHeight="1">
       <c r="C9" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="51"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="16" t="s">
         <v>54</v>
       </c>
@@ -3501,21 +3501,21 @@
       <c r="J9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="55"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="42"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="27"/>
     </row>
     <row r="10" spans="3:14" ht="14.25" customHeight="1">
       <c r="C10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="51"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="16"/>
       <c r="I10" s="14" t="s">
         <v>77</v>
@@ -3523,21 +3523,21 @@
       <c r="J10" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="45"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="3:14" ht="14.25" customHeight="1">
       <c r="C11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="51"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="16"/>
       <c r="I11" s="14" t="s">
         <v>78</v>
@@ -3545,21 +3545,21 @@
       <c r="J11" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="43"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="45"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="3:14" ht="14.25" customHeight="1">
       <c r="C12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
       <c r="H12" s="16"/>
       <c r="I12" s="14" t="s">
         <v>78</v>
@@ -3567,21 +3567,21 @@
       <c r="J12" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K12" s="43"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="45"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="3:14" ht="14.25" customHeight="1">
       <c r="C13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="16"/>
       <c r="I13" s="14" t="s">
         <v>78</v>
@@ -3589,21 +3589,21 @@
       <c r="J13" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K13" s="43"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="45"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="30"/>
     </row>
     <row r="14" spans="3:14" ht="14.25" customHeight="1">
       <c r="C14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="24"/>
       <c r="H14" s="16"/>
       <c r="I14" s="14" t="s">
         <v>78</v>
@@ -3611,21 +3611,21 @@
       <c r="J14" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K14" s="43"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="45"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" spans="3:14" ht="14.25" customHeight="1">
       <c r="C15" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="51"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="16"/>
       <c r="I15" s="14" t="s">
         <v>78</v>
@@ -3633,39 +3633,39 @@
       <c r="J15" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="K15" s="46"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="48"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="33"/>
     </row>
     <row r="16" spans="3:14" ht="14.25" customHeight="1">
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="52" t="s">
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="51"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="24"/>
     </row>
     <row r="17" spans="3:14" ht="14.25" customHeight="1">
       <c r="C17" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="D17" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="51"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="16" t="s">
         <v>54</v>
       </c>
@@ -3675,23 +3675,23 @@
       <c r="J17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="40" t="s">
+      <c r="K17" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="42"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="27"/>
     </row>
     <row r="18" spans="3:14" ht="14.25" customHeight="1">
       <c r="C18" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="16"/>
       <c r="I18" s="14" t="s">
         <v>78</v>
@@ -3699,21 +3699,21 @@
       <c r="J18" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="43"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="45"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="30"/>
     </row>
     <row r="19" spans="3:14" ht="14.25" customHeight="1">
       <c r="C19" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="16" t="s">
         <v>20</v>
       </c>
@@ -3723,21 +3723,21 @@
       <c r="J19" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="K19" s="43"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="45"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="30"/>
     </row>
     <row r="20" spans="3:14" ht="14.25" customHeight="1">
       <c r="C20" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="51"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="16"/>
       <c r="I20" s="14" t="s">
         <v>77</v>
@@ -3745,21 +3745,21 @@
       <c r="J20" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="43"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="45"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="30"/>
     </row>
     <row r="21" spans="3:14" ht="14.25" customHeight="1">
       <c r="C21" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="16"/>
       <c r="I21" s="14" t="s">
         <v>77</v>
@@ -3767,21 +3767,21 @@
       <c r="J21" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="K21" s="43"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="45"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="30"/>
     </row>
     <row r="22" spans="3:14" ht="14.25" customHeight="1">
       <c r="C22" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="51"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="24"/>
       <c r="H22" s="16"/>
       <c r="I22" s="14" t="s">
         <v>78</v>
@@ -3789,21 +3789,21 @@
       <c r="J22" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K22" s="43"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="45"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="30"/>
     </row>
     <row r="23" spans="3:14" ht="14.25" customHeight="1">
       <c r="C23" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="51"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="16"/>
       <c r="I23" s="14" t="s">
         <v>78</v>
@@ -3811,21 +3811,21 @@
       <c r="J23" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K23" s="43"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="45"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="30"/>
     </row>
     <row r="24" spans="3:14" ht="14.25" customHeight="1">
       <c r="C24" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="51"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="24"/>
       <c r="H24" s="16"/>
       <c r="I24" s="14" t="s">
         <v>75</v>
@@ -3833,39 +3833,39 @@
       <c r="J24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K24" s="46"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="48"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="33"/>
     </row>
     <row r="25" spans="3:14" ht="14.25" customHeight="1">
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="52" t="s">
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L25" s="50"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="51"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="24"/>
     </row>
     <row r="26" spans="3:14" ht="14.25" customHeight="1">
       <c r="C26" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="52" t="s">
+      <c r="D26" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="51"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="24"/>
       <c r="H26" s="16" t="s">
         <v>54</v>
       </c>
@@ -3875,21 +3875,21 @@
       <c r="J26" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="53"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="42"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="27"/>
     </row>
     <row r="27" spans="3:14" ht="14.25" customHeight="1">
       <c r="C27" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="49" t="s">
+      <c r="D27" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="51"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="24"/>
       <c r="H27" s="16"/>
       <c r="I27" s="14" t="s">
         <v>75</v>
@@ -3897,21 +3897,21 @@
       <c r="J27" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="K27" s="43"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="45"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="30"/>
     </row>
     <row r="28" spans="3:14" ht="14.25" customHeight="1">
       <c r="C28" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="51"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="16"/>
       <c r="I28" s="14" t="s">
         <v>75</v>
@@ -3919,21 +3919,21 @@
       <c r="J28" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="K28" s="43"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="45"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="30"/>
     </row>
     <row r="29" spans="3:14" ht="14.25" customHeight="1">
       <c r="C29" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="49" t="s">
+      <c r="D29" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="51"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="24"/>
       <c r="H29" s="16"/>
       <c r="I29" s="14" t="s">
         <v>76</v>
@@ -3941,21 +3941,21 @@
       <c r="J29" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K29" s="43"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="45"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="30"/>
     </row>
     <row r="30" spans="3:14" ht="14.25" customHeight="1">
       <c r="C30" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="49" t="s">
+      <c r="D30" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="51"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="24"/>
       <c r="H30" s="16"/>
       <c r="I30" s="14" t="s">
         <v>75</v>
@@ -3963,39 +3963,39 @@
       <c r="J30" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K30" s="46"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="48"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="33"/>
     </row>
     <row r="31" spans="3:14" ht="14.25" customHeight="1">
-      <c r="C31" s="52" t="s">
+      <c r="C31" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="52" t="s">
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="51"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="24"/>
     </row>
     <row r="32" spans="3:14" ht="14.25" customHeight="1">
       <c r="C32" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="52" t="s">
+      <c r="D32" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="51"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="24"/>
       <c r="H32" s="16" t="s">
         <v>54</v>
       </c>
@@ -4005,42 +4005,42 @@
       <c r="J32" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="53"/>
-      <c r="L32" s="41"/>
-      <c r="M32" s="41"/>
-      <c r="N32" s="42"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="27"/>
     </row>
     <row r="33" spans="3:14" ht="14.25" customHeight="1">
       <c r="C33" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="49"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="51"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
       <c r="H33" s="16"/>
       <c r="I33" s="14"/>
       <c r="J33" s="18"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="44"/>
-      <c r="M33" s="44"/>
-      <c r="N33" s="45"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="30"/>
     </row>
     <row r="34" spans="3:14" ht="14.25" customHeight="1">
       <c r="C34" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="49"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="51"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
       <c r="H34" s="16"/>
       <c r="I34" s="14"/>
       <c r="J34" s="18"/>
-      <c r="K34" s="46"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="48"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="33"/>
     </row>
     <row r="35" spans="3:14" ht="14.25" customHeight="1"/>
     <row r="36" spans="3:14" ht="14.25" customHeight="1"/>
@@ -5010,12 +5010,22 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="K31:N31"/>
-    <mergeCell ref="K32:N34"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="K17:N24"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="K26:N30"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D30:G30"/>
     <mergeCell ref="D15:G15"/>
     <mergeCell ref="D17:G17"/>
     <mergeCell ref="D3:N3"/>
@@ -5032,22 +5042,12 @@
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="C16:J16"/>
     <mergeCell ref="K16:N16"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="K26:N30"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="K17:N24"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="K31:N31"/>
+    <mergeCell ref="K32:N34"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D34:G34"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I10:I15 I18:I24 I27:I30 I33:I34" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -5067,7 +5067,7 @@
   <dimension ref="C4:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5084,67 +5084,67 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:14" ht="15.75">
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="51"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24"/>
     </row>
     <row r="5" spans="3:14" ht="15.75">
       <c r="C5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="51"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="24"/>
     </row>
     <row r="6" spans="3:14" ht="15.75">
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="52" t="s">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="51"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="24"/>
     </row>
     <row r="7" spans="3:14" ht="15.75">
       <c r="C7" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="51"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="16" t="s">
         <v>54</v>
       </c>
@@ -5154,21 +5154,21 @@
       <c r="J7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="55"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="42"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="27"/>
     </row>
     <row r="8" spans="3:14" ht="15.75">
       <c r="C8" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="51"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="16"/>
       <c r="I8" s="14" t="s">
         <v>78</v>
@@ -5176,21 +5176,21 @@
       <c r="J8" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="43"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="45"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="30"/>
     </row>
     <row r="9" spans="3:14" ht="15.75">
       <c r="C9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="51"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="16"/>
       <c r="I9" s="14" t="s">
         <v>78</v>
@@ -5198,21 +5198,21 @@
       <c r="J9" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="43"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="45"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="30"/>
     </row>
     <row r="10" spans="3:14" ht="15.75">
       <c r="C10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="51"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="16" t="s">
         <v>26</v>
       </c>
@@ -5222,21 +5222,21 @@
       <c r="J10" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="45"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="3:14" ht="15.75">
       <c r="C11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="51"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="16"/>
       <c r="I11" s="14" t="s">
         <v>75</v>
@@ -5244,21 +5244,21 @@
       <c r="J11" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K11" s="43"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="45"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="3:14" ht="15.75">
       <c r="C12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
       <c r="H12" s="16" t="s">
         <v>39</v>
       </c>
@@ -5268,21 +5268,21 @@
       <c r="J12" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K12" s="43"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="45"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="3:14" ht="15.75">
       <c r="C13" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="16"/>
       <c r="I13" s="14" t="s">
         <v>77</v>
@@ -5290,39 +5290,39 @@
       <c r="J13" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K13" s="46"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="48"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="33"/>
     </row>
     <row r="14" spans="3:14" ht="15.75">
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="52" t="s">
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="51"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="24"/>
     </row>
     <row r="15" spans="3:14" ht="15.75">
       <c r="C15" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="51"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="16" t="s">
         <v>54</v>
       </c>
@@ -5332,21 +5332,21 @@
       <c r="J15" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="40"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="42"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="27"/>
     </row>
     <row r="16" spans="3:14" ht="15.75">
       <c r="C16" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="51"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="16"/>
       <c r="I16" s="14" t="s">
         <v>76</v>
@@ -5354,21 +5354,21 @@
       <c r="J16" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="K16" s="43"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="45"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="30"/>
     </row>
     <row r="17" spans="3:14" ht="15.75">
       <c r="C17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="51"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="16"/>
       <c r="I17" s="14" t="s">
         <v>75</v>
@@ -5376,21 +5376,21 @@
       <c r="J17" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K17" s="43"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
-      <c r="N17" s="45"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="30"/>
     </row>
     <row r="18" spans="3:14" ht="15.75">
       <c r="C18" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="16"/>
       <c r="I18" s="14" t="s">
         <v>76</v>
@@ -5398,21 +5398,21 @@
       <c r="J18" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K18" s="43"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="45"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="30"/>
     </row>
     <row r="19" spans="3:14" ht="15.75">
       <c r="C19" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="16" t="s">
         <v>26</v>
       </c>
@@ -5422,21 +5422,21 @@
       <c r="J19" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="43"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="45"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="30"/>
     </row>
     <row r="20" spans="3:14" ht="15.75">
       <c r="C20" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="51"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="16" t="s">
         <v>26</v>
       </c>
@@ -5446,21 +5446,21 @@
       <c r="J20" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K20" s="43"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="45"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="30"/>
     </row>
     <row r="21" spans="3:14" ht="15.75">
       <c r="C21" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="16"/>
       <c r="I21" s="14" t="s">
         <v>75</v>
@@ -5468,21 +5468,21 @@
       <c r="J21" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K21" s="43"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="45"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="30"/>
     </row>
     <row r="22" spans="3:14" ht="15.75">
       <c r="C22" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="57"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="59"/>
       <c r="H22" s="16"/>
       <c r="I22" s="14" t="s">
         <v>77</v>
@@ -5490,21 +5490,21 @@
       <c r="J22" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K22" s="43"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="45"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="30"/>
     </row>
     <row r="23" spans="3:14" ht="15.75">
       <c r="C23" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="57"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="59"/>
       <c r="H23" s="16"/>
       <c r="I23" s="14" t="s">
         <v>76</v>
@@ -5512,21 +5512,21 @@
       <c r="J23" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K23" s="43"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="45"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="30"/>
     </row>
     <row r="24" spans="3:14" ht="15.75">
-      <c r="C24" s="58" t="s">
+      <c r="C24" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="51"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="24"/>
       <c r="H24" s="16"/>
       <c r="I24" s="14" t="s">
         <v>75</v>
@@ -5534,39 +5534,39 @@
       <c r="J24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K24" s="46"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="48"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="33"/>
     </row>
     <row r="25" spans="3:14" ht="15.75">
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="52" t="s">
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L25" s="50"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="51"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="24"/>
     </row>
     <row r="26" spans="3:14" ht="15.75">
       <c r="C26" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="52" t="s">
+      <c r="D26" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="51"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="24"/>
       <c r="H26" s="16" t="s">
         <v>54</v>
       </c>
@@ -5576,21 +5576,21 @@
       <c r="J26" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="53"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="42"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="27"/>
     </row>
     <row r="27" spans="3:14" ht="15.75">
       <c r="C27" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="49" t="s">
+      <c r="D27" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="51"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="24"/>
       <c r="H27" s="16"/>
       <c r="I27" s="14" t="s">
         <v>75</v>
@@ -5598,21 +5598,21 @@
       <c r="J27" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K27" s="43"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="45"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="30"/>
     </row>
     <row r="28" spans="3:14" ht="15.75">
       <c r="C28" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="51"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="16"/>
       <c r="I28" s="14" t="s">
         <v>75</v>
@@ -5620,21 +5620,21 @@
       <c r="J28" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K28" s="43"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="45"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="30"/>
     </row>
     <row r="29" spans="3:14" ht="15.75">
       <c r="C29" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="49" t="s">
+      <c r="D29" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="51"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="24"/>
       <c r="H29" s="16"/>
       <c r="I29" s="14" t="s">
         <v>75</v>
@@ -5642,21 +5642,21 @@
       <c r="J29" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K29" s="43"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="45"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="30"/>
     </row>
     <row r="30" spans="3:14" ht="15.75">
       <c r="C30" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="49" t="s">
+      <c r="D30" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="57"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="59"/>
       <c r="H30" s="16"/>
       <c r="I30" s="14" t="s">
         <v>75</v>
@@ -5664,21 +5664,21 @@
       <c r="J30" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K30" s="43"/>
-      <c r="L30" s="44"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="45"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="30"/>
     </row>
     <row r="31" spans="3:14" ht="15.75">
       <c r="C31" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D31" s="49" t="s">
+      <c r="D31" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="51"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="24"/>
       <c r="H31" s="16"/>
       <c r="I31" s="14" t="s">
         <v>77</v>
@@ -5686,39 +5686,39 @@
       <c r="J31" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K31" s="46"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="48"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="33"/>
     </row>
     <row r="32" spans="3:14" ht="15.75">
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="51"/>
-      <c r="K32" s="59" t="s">
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="L32" s="41"/>
-      <c r="M32" s="41"/>
-      <c r="N32" s="42"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="27"/>
     </row>
     <row r="33" spans="3:14" ht="15.75">
       <c r="C33" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="52" t="s">
+      <c r="D33" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="51"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
       <c r="H33" s="16" t="s">
         <v>54</v>
       </c>
@@ -5728,145 +5728,118 @@
       <c r="J33" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="60"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="60"/>
+      <c r="K33" s="57"/>
+      <c r="L33" s="57"/>
+      <c r="M33" s="57"/>
+      <c r="N33" s="57"/>
     </row>
     <row r="34" spans="3:14" ht="15.75">
       <c r="C34" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="49" t="s">
+      <c r="D34" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="51"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
       <c r="H34" s="16"/>
       <c r="I34" s="14" t="s">
         <v>112</v>
       </c>
       <c r="J34" s="20"/>
-      <c r="K34" s="60"/>
-      <c r="L34" s="60"/>
-      <c r="M34" s="60"/>
-      <c r="N34" s="60"/>
+      <c r="K34" s="57"/>
+      <c r="L34" s="57"/>
+      <c r="M34" s="57"/>
+      <c r="N34" s="57"/>
     </row>
     <row r="35" spans="3:14" ht="15" customHeight="1">
       <c r="C35" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="49" t="s">
+      <c r="D35" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="51"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="24"/>
       <c r="H35" s="16"/>
       <c r="I35" s="14" t="s">
         <v>112</v>
       </c>
       <c r="J35" s="20"/>
-      <c r="K35" s="60"/>
-      <c r="L35" s="60"/>
-      <c r="M35" s="60"/>
-      <c r="N35" s="60"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="57"/>
+      <c r="M35" s="57"/>
+      <c r="N35" s="57"/>
     </row>
     <row r="36" spans="3:14" ht="15.75">
       <c r="C36" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="49" t="s">
+      <c r="D36" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="51"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="24"/>
       <c r="H36" s="16"/>
       <c r="I36" s="14" t="s">
         <v>112</v>
       </c>
       <c r="J36" s="20"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="60"/>
-      <c r="N36" s="60"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="57"/>
+      <c r="M36" s="57"/>
+      <c r="N36" s="57"/>
     </row>
     <row r="37" spans="3:14" ht="15.75">
       <c r="C37" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="D37" s="49" t="s">
+      <c r="D37" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="51"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="24"/>
       <c r="H37" s="16"/>
       <c r="I37" s="14" t="s">
         <v>112</v>
       </c>
       <c r="J37" s="20"/>
-      <c r="K37" s="60"/>
-      <c r="L37" s="60"/>
-      <c r="M37" s="60"/>
-      <c r="N37" s="60"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="57"/>
+      <c r="M37" s="57"/>
+      <c r="N37" s="57"/>
     </row>
     <row r="38" spans="3:14" ht="15.75">
       <c r="C38" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="49" t="s">
+      <c r="D38" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="51"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="24"/>
       <c r="H38" s="16"/>
       <c r="I38" s="14" t="s">
         <v>112</v>
       </c>
       <c r="J38" s="20"/>
-      <c r="K38" s="60"/>
-      <c r="L38" s="60"/>
-      <c r="M38" s="60"/>
-      <c r="N38" s="60"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="57"/>
+      <c r="M38" s="57"/>
+      <c r="N38" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="C4:N4"/>
-    <mergeCell ref="D5:N5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="K7:N13"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="K15:N24"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="C14:J14"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="C25:J25"/>
     <mergeCell ref="K25:N25"/>
     <mergeCell ref="D38:G38"/>
     <mergeCell ref="K33:N38"/>
     <mergeCell ref="D23:G23"/>
     <mergeCell ref="D30:G30"/>
-    <mergeCell ref="D22:G22"/>
     <mergeCell ref="D36:G36"/>
     <mergeCell ref="D37:G37"/>
     <mergeCell ref="D31:G31"/>
@@ -5878,6 +5851,33 @@
     <mergeCell ref="D26:G26"/>
     <mergeCell ref="K26:N31"/>
     <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="K15:N24"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="D5:N5"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="K7:N13"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="2">

</xml_diff>